<commit_message>
VR_Input#26　認識率が50%未満の英単語　認識テスト（再）終了 cat(28%),cow(96%),giraffe(60%),bear(8%),monkey(16%),wolf(24%),tiger(0%),lion(16%), hamburger(52%),water(20%),salmon(60%),meat(4%),candy(4%),fish(4%),yogurt(0%)となった。
</commit_message>
<xml_diff>
--- a/月読アイ　認識テスト.xlsx
+++ b/月読アイ　認識テスト.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="82">
   <si>
     <t>英単語</t>
   </si>
@@ -64,12 +64,12 @@
     <t>×　〃</t>
   </si>
   <si>
+    <t>×　horse</t>
+  </si>
+  <si>
     <t>×　(wolf）</t>
   </si>
   <si>
-    <t>×　horse</t>
-  </si>
-  <si>
     <t>×　(wolf)</t>
   </si>
   <si>
@@ -109,6 +109,15 @@
     <t>×　horse　salmon</t>
   </si>
   <si>
+    <t>×　horse　wolf</t>
+  </si>
+  <si>
+    <t>×　wolf　horse</t>
+  </si>
+  <si>
+    <t>○　同時にhorse</t>
+  </si>
+  <si>
     <t>1/2確率</t>
   </si>
   <si>
@@ -175,9 +184,15 @@
     <t>×　(salmon）</t>
   </si>
   <si>
+    <t>×　salmon</t>
+  </si>
+  <si>
     <t>×　(cat）</t>
   </si>
   <si>
+    <t>×　cat</t>
+  </si>
+  <si>
     <t>×　(bear)</t>
   </si>
   <si>
@@ -190,6 +205,12 @@
     <t>×　(cow）</t>
   </si>
   <si>
+    <t>×　candy</t>
+  </si>
+  <si>
+    <t>×　wolf　giraffe</t>
+  </si>
+  <si>
     <t>○　(同時にwolf)</t>
   </si>
   <si>
@@ -202,13 +223,28 @@
     <t>×　　　〃</t>
   </si>
   <si>
+    <t>×　horse　giraffe</t>
+  </si>
+  <si>
     <t>○　(同時にhorse）</t>
   </si>
   <si>
+    <t>×　giraffe　candy</t>
+  </si>
+  <si>
+    <t>×　cow　wolf　monkey</t>
+  </si>
+  <si>
     <t>×　(cat)</t>
   </si>
   <si>
+    <t>×　cow　wolf</t>
+  </si>
+  <si>
     <t>○　(同時にcow)</t>
+  </si>
+  <si>
+    <t>○　同時にcow</t>
   </si>
   <si>
     <t>○　　　〃</t>
@@ -335,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -356,9 +392,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -398,11 +431,14 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="3" max="3" width="26.29"/>
+    <col customWidth="1" min="4" max="4" width="19.86"/>
     <col customWidth="1" min="5" max="5" width="18.57"/>
     <col customWidth="1" min="6" max="6" width="19.71"/>
     <col customWidth="1" min="7" max="7" width="19.86"/>
     <col customWidth="1" min="8" max="8" width="17.43"/>
     <col customWidth="1" min="9" max="9" width="21.0"/>
+    <col customWidth="1" min="10" max="10" width="19.43"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -449,11 +485,11 @@
       </c>
       <c r="J4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>20%</v>
+        <v>16%</v>
       </c>
       <c r="L4" s="2" t="str">
         <f>sum(C4:J4)/8</f>
-        <v>32%</v>
+        <v>31%</v>
       </c>
     </row>
     <row r="5">
@@ -508,8 +544,12 @@
       <c r="H6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="6"/>
@@ -531,8 +571,12 @@
       <c r="H7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -546,19 +590,23 @@
         <v>13</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="G8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="6"/>
@@ -580,8 +628,12 @@
       <c r="H9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10">
@@ -602,10 +654,14 @@
         <v>13</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="8" t="s">
@@ -617,27 +673,27 @@
       <c r="D11" s="9">
         <v>1.0</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>0.8</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>0.0</v>
       </c>
       <c r="G11" s="9">
         <v>0.6</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="9">
         <v>0.6</v>
       </c>
       <c r="I11" s="9">
         <v>0.0</v>
       </c>
       <c r="J11" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="K11" s="11" t="str">
+        <v>0.4</v>
+      </c>
+      <c r="K11" s="10" t="str">
         <f>sum(C11:J11)/8</f>
-        <v>38%</v>
+        <v>43%</v>
       </c>
     </row>
     <row r="12">
@@ -657,13 +713,17 @@
         <v>24</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="6"/>
@@ -685,13 +745,17 @@
       <c r="H13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="6"/>
       <c r="C14" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>13</v>
@@ -708,8 +772,12 @@
       <c r="H14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" s="6"/>
@@ -731,8 +799,12 @@
       <c r="H15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="I15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="7"/>
@@ -754,14 +826,18 @@
       <c r="H16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="I16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="17">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>0.6</v>
       </c>
       <c r="D17" s="9">
@@ -773,7 +849,7 @@
       <c r="F17" s="9">
         <v>0.0</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="9">
         <v>0.0</v>
       </c>
       <c r="H17" s="9">
@@ -785,7 +861,7 @@
       <c r="J17" s="9">
         <v>0.0</v>
       </c>
-      <c r="K17" s="11" t="str">
+      <c r="K17" s="10" t="str">
         <f>sum(C17:J17)/8</f>
         <v>20%</v>
       </c>
@@ -812,8 +888,12 @@
       <c r="H18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
+      <c r="I18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="6"/>
@@ -835,8 +915,12 @@
       <c r="H19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="I19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="6"/>
@@ -853,13 +937,17 @@
         <v>25</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" s="6"/>
@@ -881,8 +969,12 @@
       <c r="H21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="I21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22">
       <c r="B22" s="7"/>
@@ -899,17 +991,21 @@
         <v>25</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="I22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="23">
-      <c r="B23" s="12" t="s">
-        <v>32</v>
+      <c r="B23" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C23" s="9">
         <v>0.8</v>
@@ -920,13 +1016,13 @@
       <c r="E23" s="9">
         <v>0.8</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="9">
         <v>0.0</v>
       </c>
       <c r="G23" s="9">
         <v>0.0</v>
       </c>
-      <c r="H23" s="10">
+      <c r="H23" s="9">
         <v>0.4</v>
       </c>
       <c r="I23" s="9">
@@ -935,40 +1031,44 @@
       <c r="J23" s="9">
         <v>0.4</v>
       </c>
-      <c r="K23" s="11" t="str">
+      <c r="K23" s="10" t="str">
         <f>sum(C23:J23)/8</f>
         <v>43%</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="G24" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="6"/>
       <c r="C25" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>13</v>
@@ -983,10 +1083,14 @@
         <v>16</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26">
       <c r="B26" s="6"/>
@@ -1008,13 +1112,17 @@
       <c r="H26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
+      <c r="I26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27">
       <c r="B27" s="6"/>
       <c r="C27" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>13</v>
@@ -1023,16 +1131,20 @@
         <v>13</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" s="7"/>
@@ -1049,17 +1161,21 @@
         <v>14</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="I28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29">
-      <c r="B29" s="12" t="s">
-        <v>38</v>
+      <c r="B29" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="C29" s="9">
         <v>0.0</v>
@@ -1067,7 +1183,7 @@
       <c r="D29" s="9">
         <v>0.8</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="9">
         <v>0.8</v>
       </c>
       <c r="F29" s="9">
@@ -1076,23 +1192,23 @@
       <c r="G29" s="9">
         <v>0.2</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29" s="9">
         <v>0.2</v>
       </c>
       <c r="I29" s="9">
         <v>0.0</v>
       </c>
       <c r="J29" s="9">
-        <v>0.4</v>
-      </c>
-      <c r="K29" s="11" t="str">
+        <v>0.0</v>
+      </c>
+      <c r="K29" s="10" t="str">
         <f>sum(C29:J29)/8</f>
-        <v>33%</v>
+        <v>28%</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>26</v>
@@ -1107,13 +1223,17 @@
         <v>14</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" s="6"/>
@@ -1124,7 +1244,7 @@
         <v>13</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>16</v>
@@ -1135,13 +1255,17 @@
       <c r="H31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="I31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="32">
       <c r="B32" s="6"/>
       <c r="C32" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>13</v>
@@ -1153,18 +1277,22 @@
         <v>13</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
+      <c r="I32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="33">
       <c r="B33" s="6"/>
       <c r="C33" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>13</v>
@@ -1176,13 +1304,17 @@
         <v>14</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
+      <c r="I33" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" s="7"/>
@@ -1199,17 +1331,21 @@
         <v>16</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
+      <c r="I34" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="35">
-      <c r="B35" s="12" t="s">
-        <v>44</v>
+      <c r="B35" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="C35" s="9">
         <v>0.0</v>
@@ -1217,13 +1353,13 @@
       <c r="D35" s="9">
         <v>1.0</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="9">
         <v>0.6</v>
       </c>
-      <c r="F35" s="10">
+      <c r="F35" s="9">
         <v>0.2</v>
       </c>
-      <c r="G35" s="10">
+      <c r="G35" s="9">
         <v>0.0</v>
       </c>
       <c r="H35" s="9">
@@ -1233,42 +1369,42 @@
         <v>0.0</v>
       </c>
       <c r="J35" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K35" s="11" t="str">
+        <v>0.0</v>
+      </c>
+      <c r="K35" s="10" t="str">
         <f>sum(C35:J35)/8</f>
-        <v>25%</v>
+        <v>23%</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="11" t="str">
+        <v>48</v>
+      </c>
+      <c r="C38" s="10" t="str">
         <f t="shared" ref="C38:I38" si="2">sum(C45,C51,C57,C63,C69)/5</f>
-        <v>48%</v>
-      </c>
-      <c r="D38" s="11" t="str">
+        <v>52%</v>
+      </c>
+      <c r="D38" s="10" t="str">
         <f t="shared" si="2"/>
         <v>20%</v>
       </c>
-      <c r="E38" s="11" t="str">
+      <c r="E38" s="10" t="str">
         <f t="shared" si="2"/>
         <v>60%</v>
       </c>
-      <c r="F38" s="11" t="str">
+      <c r="F38" s="10" t="str">
         <f t="shared" si="2"/>
         <v>4%</v>
       </c>
-      <c r="G38" s="11" t="str">
+      <c r="G38" s="10" t="str">
         <f t="shared" si="2"/>
         <v>4%</v>
       </c>
-      <c r="H38" s="11" t="str">
+      <c r="H38" s="10" t="str">
         <f t="shared" si="2"/>
         <v>4%</v>
       </c>
-      <c r="I38" s="11" t="str">
+      <c r="I38" s="10" t="str">
         <f t="shared" si="2"/>
         <v>0%</v>
       </c>
@@ -1276,27 +1412,27 @@
     <row r="39">
       <c r="B39" s="3"/>
       <c r="C39" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I39" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="J39" s="14"/>
+        <v>54</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J39" s="13"/>
     </row>
     <row r="40">
       <c r="B40" s="5" t="s">
@@ -1306,7 +1442,7 @@
         <v>13</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>13</v>
@@ -1318,12 +1454,12 @@
         <v>23</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I40" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I40" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J40" s="15"/>
+      <c r="J40" s="14"/>
     </row>
     <row r="41">
       <c r="B41" s="6"/>
@@ -1331,7 +1467,7 @@
         <v>13</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>13</v>
@@ -1345,10 +1481,10 @@
       <c r="H41" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I41" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="J41" s="15"/>
+      <c r="I41" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J41" s="14"/>
     </row>
     <row r="42">
       <c r="B42" s="6"/>
@@ -1356,7 +1492,7 @@
         <v>15</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>15</v>
@@ -1370,10 +1506,10 @@
       <c r="H42" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I42" s="13" t="s">
+      <c r="I42" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J42" s="15"/>
+      <c r="J42" s="14"/>
     </row>
     <row r="43">
       <c r="B43" s="6"/>
@@ -1381,13 +1517,13 @@
         <v>13</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>25</v>
@@ -1395,10 +1531,10 @@
       <c r="H43" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I43" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J43" s="15"/>
+      <c r="I43" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J43" s="14"/>
     </row>
     <row r="44">
       <c r="B44" s="7"/>
@@ -1406,7 +1542,7 @@
         <v>15</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>13</v>
@@ -1420,13 +1556,13 @@
       <c r="H44" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I44" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J44" s="15"/>
+      <c r="I44" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J44" s="14"/>
     </row>
     <row r="45">
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C45" s="9">
@@ -1435,7 +1571,7 @@
       <c r="D45" s="9">
         <v>0.0</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="9">
         <v>0.6</v>
       </c>
       <c r="F45" s="9">
@@ -1447,10 +1583,10 @@
       <c r="H45" s="9">
         <v>0.0</v>
       </c>
-      <c r="I45" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="J45" s="17" t="str">
+      <c r="I45" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="J45" s="16" t="str">
         <f>sum(C45:I45)/7</f>
         <v>17%</v>
       </c>
@@ -1463,13 +1599,13 @@
         <v>13</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>23</v>
@@ -1477,10 +1613,10 @@
       <c r="H46" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="J46" s="15"/>
+      <c r="I46" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J46" s="14"/>
     </row>
     <row r="47">
       <c r="B47" s="6"/>
@@ -1488,7 +1624,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>15</v>
@@ -1500,12 +1636,12 @@
         <v>16</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I47" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="J47" s="15"/>
+        <v>56</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J47" s="14"/>
     </row>
     <row r="48">
       <c r="B48" s="6"/>
@@ -1513,7 +1649,7 @@
         <v>13</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>13</v>
@@ -1522,15 +1658,15 @@
         <v>25</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I48" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="J48" s="15"/>
+      <c r="I48" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J48" s="14"/>
     </row>
     <row r="49">
       <c r="B49" s="6"/>
@@ -1538,7 +1674,7 @@
         <v>15</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>15</v>
@@ -1552,10 +1688,10 @@
       <c r="H49" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I49" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="J49" s="15"/>
+      <c r="I49" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J49" s="14"/>
     </row>
     <row r="50">
       <c r="B50" s="7"/>
@@ -1563,7 +1699,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>15</v>
@@ -1577,39 +1713,39 @@
       <c r="H50" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I50" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J50" s="15"/>
+      <c r="I50" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J50" s="14"/>
     </row>
     <row r="51">
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C51" s="9">
         <v>0.8</v>
       </c>
       <c r="D51" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="E51" s="10">
         <v>0.2</v>
       </c>
+      <c r="E51" s="9">
+        <v>0.2</v>
+      </c>
       <c r="F51" s="9">
         <v>0.0</v>
       </c>
-      <c r="G51" s="10">
+      <c r="G51" s="9">
         <v>0.2</v>
       </c>
-      <c r="H51" s="10">
+      <c r="H51" s="9">
         <v>0.2</v>
       </c>
-      <c r="I51" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="J51" s="17" t="str">
+      <c r="I51" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="J51" s="16" t="str">
         <f>sum(C51:I51)/7</f>
-        <v>20%</v>
+        <v>23%</v>
       </c>
     </row>
     <row r="52">
@@ -1617,13 +1753,13 @@
         <v>29</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>23</v>
@@ -1632,26 +1768,26 @@
         <v>23</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I52" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="J52" s="15"/>
+        <v>56</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J52" s="14"/>
     </row>
     <row r="53">
       <c r="B53" s="6"/>
       <c r="C53" s="4" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>16</v>
@@ -1659,24 +1795,24 @@
       <c r="H53" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I53" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J53" s="15"/>
+      <c r="I53" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J53" s="14"/>
     </row>
     <row r="54">
       <c r="B54" s="6"/>
       <c r="C54" s="4" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>16</v>
@@ -1684,21 +1820,21 @@
       <c r="H54" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I54" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="J54" s="15"/>
+      <c r="I54" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J54" s="14"/>
     </row>
     <row r="55">
       <c r="B55" s="6"/>
       <c r="C55" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>23</v>
@@ -1709,24 +1845,24 @@
       <c r="H55" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I55" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="J55" s="15"/>
+      <c r="I55" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J55" s="14"/>
     </row>
     <row r="56">
       <c r="B56" s="7"/>
       <c r="C56" s="4" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>16</v>
@@ -1734,14 +1870,14 @@
       <c r="H56" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I56" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="J56" s="15"/>
+      <c r="I56" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J56" s="14"/>
     </row>
     <row r="57">
-      <c r="B57" s="12" t="s">
-        <v>32</v>
+      <c r="B57" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C57" s="9">
         <v>0.0</v>
@@ -1749,10 +1885,10 @@
       <c r="D57" s="9">
         <v>0.0</v>
       </c>
-      <c r="E57" s="10">
+      <c r="E57" s="9">
         <v>1.0</v>
       </c>
-      <c r="F57" s="10">
+      <c r="F57" s="9">
         <v>0.2</v>
       </c>
       <c r="G57" s="9">
@@ -1761,23 +1897,23 @@
       <c r="H57" s="9">
         <v>0.0</v>
       </c>
-      <c r="I57" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="J57" s="17" t="str">
+      <c r="I57" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="J57" s="16" t="str">
         <f>sum(C57:I57)/7</f>
         <v>17%</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>15</v>
@@ -1789,26 +1925,26 @@
         <v>23</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I58" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J58" s="15"/>
+        <v>56</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J58" s="14"/>
     </row>
     <row r="59">
       <c r="B59" s="6"/>
       <c r="C59" s="4" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>16</v>
@@ -1816,24 +1952,24 @@
       <c r="H59" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I59" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J59" s="15"/>
+      <c r="I59" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J59" s="14"/>
     </row>
     <row r="60">
       <c r="B60" s="6"/>
       <c r="C60" s="4" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>16</v>
@@ -1841,24 +1977,24 @@
       <c r="H60" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I60" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J60" s="15"/>
+      <c r="I60" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J60" s="14"/>
     </row>
     <row r="61">
       <c r="B61" s="6"/>
       <c r="C61" s="4" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>16</v>
@@ -1866,24 +2002,24 @@
       <c r="H61" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I61" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J61" s="15"/>
+      <c r="I61" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J61" s="14"/>
     </row>
     <row r="62">
       <c r="B62" s="7"/>
       <c r="C62" s="4" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>16</v>
@@ -1891,22 +2027,22 @@
       <c r="H62" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I62" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J62" s="15"/>
+      <c r="I62" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J62" s="14"/>
     </row>
     <row r="63">
-      <c r="B63" s="12" t="s">
-        <v>38</v>
+      <c r="B63" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="C63" s="9">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D63" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E63" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="E63" s="9">
         <v>0.8</v>
       </c>
       <c r="F63" s="9">
@@ -1918,17 +2054,17 @@
       <c r="H63" s="9">
         <v>0.0</v>
       </c>
-      <c r="I63" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="J63" s="17" t="str">
+      <c r="I63" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="J63" s="16" t="str">
         <f>sum(C63:I63)/7</f>
         <v>20%</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>15</v>
@@ -1943,15 +2079,15 @@
         <v>23</v>
       </c>
       <c r="G64" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H64" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H64" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I64" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="J64" s="15"/>
+      <c r="I64" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J64" s="14"/>
     </row>
     <row r="65">
       <c r="B65" s="6"/>
@@ -1962,10 +2098,10 @@
         <v>15</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>26</v>
@@ -1973,10 +2109,10 @@
       <c r="H65" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I65" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="J65" s="15"/>
+      <c r="I65" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J65" s="14"/>
     </row>
     <row r="66">
       <c r="B66" s="6"/>
@@ -1990,18 +2126,18 @@
         <v>15</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="H66" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I66" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="J66" s="15"/>
+      <c r="I66" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J66" s="14"/>
     </row>
     <row r="67">
       <c r="B67" s="6"/>
@@ -2012,21 +2148,21 @@
         <v>13</v>
       </c>
       <c r="E67" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G67" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F67" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="H67" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I67" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="J67" s="15"/>
+      <c r="I67" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J67" s="14"/>
     </row>
     <row r="68">
       <c r="B68" s="7"/>
@@ -2040,7 +2176,7 @@
         <v>15</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>23</v>
@@ -2048,14 +2184,14 @@
       <c r="H68" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I68" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="J68" s="15"/>
+      <c r="I68" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J68" s="14"/>
     </row>
     <row r="69">
-      <c r="B69" s="18" t="s">
-        <v>44</v>
+      <c r="B69" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="C69" s="9">
         <v>0.6</v>
@@ -2063,7 +2199,7 @@
       <c r="D69" s="9">
         <v>0.8</v>
       </c>
-      <c r="E69" s="10">
+      <c r="E69" s="9">
         <v>0.4</v>
       </c>
       <c r="F69" s="9">
@@ -2078,7 +2214,7 @@
       <c r="I69" s="9">
         <v>0.0</v>
       </c>
-      <c r="J69" s="17" t="str">
+      <c r="J69" s="16" t="str">
         <f>sum(C69:I69)/7</f>
         <v>26%</v>
       </c>

</xml_diff>